<commit_message>
5 familias de restricciones
Actualizado el algoritmo para construir las primeras 5 familias de restricciones, hasta evitar solapamiento de cultivos.
</commit_message>
<xml_diff>
--- a/Productos.xlsx
+++ b/Productos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEONARDO\Dropbox\00 MAESTRIA\02-01 Modelo\00 FINAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Dropbox\00 MAESTRIA\02-01 Modelo\00 FINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,8 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="36">
   <si>
     <t>Ahuyama</t>
   </si>
@@ -118,11 +119,26 @@
   <si>
     <t/>
   </si>
+  <si>
+    <t>Gv</t>
+  </si>
+  <si>
+    <t>Frutas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verduras y Hortalizas</t>
+  </si>
+  <si>
+    <t>Tubérculos, raíces y plátanos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Otros grupos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -570,7 +586,7 @@
   <dimension ref="A1:FB57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +594,7 @@
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="4"/>
+    <col min="4" max="4" width="29.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
@@ -601,7 +617,12 @@
       <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -765,7 +786,13 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="D2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="4">
+        <f>+VLOOKUP(D2,$G$29:$H$32,2,FALSE)</f>
+        <v>2</v>
+      </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
@@ -816,7 +843,13 @@
       <c r="C3" s="4">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="D3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E22" si="0">+VLOOKUP(D3,$G$29:$H$32,2,FALSE)</f>
+        <v>3</v>
+      </c>
       <c r="F3" s="5">
         <v>1</v>
       </c>
@@ -918,91 +951,91 @@
         <v>,0,0,0,0</v>
       </c>
       <c r="AN3" s="5" t="str">
-        <f t="shared" ref="AN3:BI14" si="0">+IF(P3="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AN3:BI14" si="1">+IF(P3="",",0,0,0,0",",1,1,1,1")</f>
         <v>,1,1,1,1</v>
       </c>
       <c r="AO3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AP3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AQ3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AR3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AS3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AT3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AU3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AV3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AW3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AX3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AY3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AZ3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BA3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BB3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BC3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BD3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BE3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BF3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BG3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BH3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BI3" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BJ3" s="22" t="str">
@@ -1308,7 +1341,13 @@
       <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="D4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="F4" s="5">
         <v>2</v>
       </c>
@@ -1400,103 +1439,103 @@
         <v>30</v>
       </c>
       <c r="AL4" s="5" t="str">
-        <f t="shared" ref="AL4:AL27" si="1">+IF(N4="","0,0,0,0","1,1,1,1")</f>
+        <f t="shared" ref="AL4:AL27" si="2">+IF(N4="","0,0,0,0","1,1,1,1")</f>
         <v>0,0,0,0</v>
       </c>
       <c r="AM4" s="5" t="str">
-        <f t="shared" ref="AM4:AM27" si="2">+IF(O4="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AM4:AM27" si="3">+IF(O4="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="AN4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AO4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AP4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AQ4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AR4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AS4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AT4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AU4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AV4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AW4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AX4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AY4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AZ4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BA4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BB4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BC4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BD4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BE4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BF4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BG4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BH4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BI4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BJ4" s="22" t="str">
-        <f t="shared" ref="BJ4:BJ27" si="3">+CONCATENATE(AL4,AM4,AN4,AO4,AP4,AQ4,AR4,AS4,AT4,AU4,AV4,AW4,AX4,AY4,AZ4,BA4,BB4,BC4,BD4,BE4,BF4,BG4,BH4,BI4)</f>
+        <f t="shared" ref="BJ4:BJ27" si="4">+CONCATENATE(AL4,AM4,AN4,AO4,AP4,AQ4,AR4,AS4,AT4,AU4,AV4,AW4,AX4,AY4,AZ4,BA4,BB4,BC4,BD4,BE4,BF4,BG4,BH4,BI4)</f>
         <v>0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK4">
@@ -1798,7 +1837,13 @@
       <c r="C5" s="4">
         <v>4</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="D5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F5" s="5">
         <v>3</v>
       </c>
@@ -1868,103 +1913,103 @@
       <c r="AJ5" s="15"/>
       <c r="AK5" s="16"/>
       <c r="AL5" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0,0,0,0</v>
       </c>
       <c r="AM5" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AN5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AO5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AP5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AQ5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AR5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AS5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AT5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AU5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AV5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AW5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AX5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AY5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AZ5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BA5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BB5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BC5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BD5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BE5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BF5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BG5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BH5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BI5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BJ5" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK5">
@@ -2266,7 +2311,13 @@
       <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="D6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="F6" s="5">
         <v>4</v>
       </c>
@@ -2354,103 +2405,103 @@
         <v>30</v>
       </c>
       <c r="AL6" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0,0,0,0</v>
       </c>
       <c r="AM6" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AN6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AO6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AP6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AQ6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AR6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AS6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AT6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AU6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AV6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AW6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AX6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AY6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AZ6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BA6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BB6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BC6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BD6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BE6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BF6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BG6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BH6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BI6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BJ6" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK6">
@@ -2752,7 +2803,13 @@
       <c r="C7" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="F7" s="5">
         <v>5</v>
       </c>
@@ -2816,103 +2873,103 @@
       <c r="AJ7" s="15"/>
       <c r="AK7" s="16"/>
       <c r="AL7" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1,1,1,1</v>
       </c>
       <c r="AM7" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AN7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AO7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AP7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AQ7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AR7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AS7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AT7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AU7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AV7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AW7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AX7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AY7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AZ7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BA7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BB7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BC7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BD7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BE7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BF7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BG7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BH7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BI7" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BJ7" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK7">
@@ -3214,7 +3271,13 @@
       <c r="C8" s="4">
         <v>1</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="D8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="F8" s="5">
         <v>6</v>
       </c>
@@ -3302,103 +3365,103 @@
         <v>30</v>
       </c>
       <c r="AL8" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0,0,0,0</v>
       </c>
       <c r="AM8" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AN8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AO8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AP8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AQ8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AR8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AS8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AT8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AU8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AV8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AW8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AX8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AY8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AZ8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BA8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BB8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BC8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BD8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BE8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BF8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BG8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BH8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BI8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BJ8" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK8">
@@ -3700,7 +3763,13 @@
       <c r="C9" s="4">
         <v>5</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="D9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="F9" s="5">
         <v>7</v>
       </c>
@@ -3792,103 +3861,103 @@
         <v>30</v>
       </c>
       <c r="AL9" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0,0,0,0</v>
       </c>
       <c r="AM9" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AN9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AO9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AP9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AQ9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AR9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AS9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AT9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AU9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AV9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AW9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AX9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AY9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AZ9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BA9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BB9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BC9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BD9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BE9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BF9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BG9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BH9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BI9" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BJ9" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK9">
@@ -4190,7 +4259,13 @@
       <c r="C10" s="4">
         <v>2</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="D10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="F10" s="5">
         <v>8</v>
       </c>
@@ -4284,103 +4359,103 @@
         <v>30</v>
       </c>
       <c r="AL10" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0,0,0,0</v>
       </c>
       <c r="AM10" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AN10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AO10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AP10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AQ10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AR10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AS10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AT10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AU10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AV10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AW10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AX10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AY10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AZ10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BA10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BB10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BC10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BD10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BE10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BF10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BG10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BH10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BI10" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BJ10" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK10">
@@ -4682,7 +4757,13 @@
       <c r="C11" s="4">
         <v>1</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="D11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="F11" s="5">
         <v>9</v>
       </c>
@@ -4776,103 +4857,103 @@
         <v>30</v>
       </c>
       <c r="AL11" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0,0,0,0</v>
       </c>
       <c r="AM11" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AN11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AO11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AP11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AQ11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AR11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AS11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AT11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AU11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AV11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AW11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AX11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AY11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AZ11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BA11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BB11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BC11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BD11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BE11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BF11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BG11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BH11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BI11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BJ11" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK11">
@@ -5174,7 +5255,13 @@
       <c r="C12" s="4">
         <v>1</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="D12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="F12" s="5">
         <v>10</v>
       </c>
@@ -5264,103 +5351,103 @@
       <c r="AJ12" s="15"/>
       <c r="AK12" s="16"/>
       <c r="AL12" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0,0,0,0</v>
       </c>
       <c r="AM12" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AN12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AO12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AP12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AQ12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AR12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AS12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AT12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AU12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AV12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AW12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AX12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AY12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AZ12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BA12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BB12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BC12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BD12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BE12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BF12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BG12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BH12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BI12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BJ12" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK12">
@@ -5662,7 +5749,13 @@
       <c r="C13" s="4">
         <v>1</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="D13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="F13" s="5">
         <v>11</v>
       </c>
@@ -5748,103 +5841,103 @@
       <c r="AJ13" s="15"/>
       <c r="AK13" s="16"/>
       <c r="AL13" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1,1,1,1</v>
       </c>
       <c r="AM13" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AN13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AO13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AP13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AQ13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AR13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AS13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AT13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AU13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AV13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AW13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AX13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AY13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AZ13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BA13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BB13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BC13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BD13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BE13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BF13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BG13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BH13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BI13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="BJ13" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK13">
@@ -6146,7 +6239,13 @@
       <c r="C14" s="4">
         <v>4</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="D14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F14" s="5">
         <v>12</v>
       </c>
@@ -6240,103 +6339,103 @@
         <v>30</v>
       </c>
       <c r="AL14" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1,1,1,1</v>
       </c>
       <c r="AM14" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AN14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AO14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AP14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AQ14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AR14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AS14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AT14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AU14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AV14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AW14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AX14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AY14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AZ14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="BA14" s="5" t="str">
-        <f t="shared" ref="BA14:BA27" si="4">+IF(AC14="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="BA14:BA27" si="5">+IF(AC14="",",0,0,0,0",",1,1,1,1")</f>
         <v>,1,1,1,1</v>
       </c>
       <c r="BB14" s="5" t="str">
-        <f t="shared" ref="BB14:BB27" si="5">+IF(AD14="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="BB14:BB27" si="6">+IF(AD14="",",0,0,0,0",",1,1,1,1")</f>
         <v>,1,1,1,1</v>
       </c>
       <c r="BC14" s="5" t="str">
-        <f t="shared" ref="BC14:BC27" si="6">+IF(AE14="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="BC14:BC27" si="7">+IF(AE14="",",0,0,0,0",",1,1,1,1")</f>
         <v>,1,1,1,1</v>
       </c>
       <c r="BD14" s="5" t="str">
-        <f t="shared" ref="BD14:BD27" si="7">+IF(AF14="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="BD14:BD27" si="8">+IF(AF14="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="BE14" s="5" t="str">
-        <f t="shared" ref="BE14:BE27" si="8">+IF(AG14="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="BE14:BE27" si="9">+IF(AG14="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="BF14" s="5" t="str">
-        <f t="shared" ref="BF14:BF27" si="9">+IF(AH14="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="BF14:BF27" si="10">+IF(AH14="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="BG14" s="5" t="str">
-        <f t="shared" ref="BG14:BG27" si="10">+IF(AI14="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="BG14:BG27" si="11">+IF(AI14="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="BH14" s="5" t="str">
-        <f t="shared" ref="BH14:BH27" si="11">+IF(AJ14="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="BH14:BH27" si="12">+IF(AJ14="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="BI14" s="5" t="str">
-        <f t="shared" ref="BI14:BI27" si="12">+IF(AK14="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="BI14:BI27" si="13">+IF(AK14="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="BJ14" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK14">
@@ -6638,7 +6737,13 @@
       <c r="C15" s="4">
         <v>3</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="F15" s="5">
         <v>13</v>
       </c>
@@ -6732,103 +6837,103 @@
         <v>30</v>
       </c>
       <c r="AL15" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0,0,0,0</v>
       </c>
       <c r="AM15" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AN15" s="5" t="str">
-        <f t="shared" ref="AN15:AN27" si="13">+IF(P15="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AN15:AN27" si="14">+IF(P15="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="AO15" s="5" t="str">
-        <f t="shared" ref="AO15:AO27" si="14">+IF(Q15="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AO15:AO27" si="15">+IF(Q15="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="AP15" s="5" t="str">
-        <f t="shared" ref="AP15:AP27" si="15">+IF(R15="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AP15:AP27" si="16">+IF(R15="",",0,0,0,0",",1,1,1,1")</f>
         <v>,1,1,1,1</v>
       </c>
       <c r="AQ15" s="5" t="str">
-        <f t="shared" ref="AQ15:AQ27" si="16">+IF(S15="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AQ15:AQ27" si="17">+IF(S15="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="AR15" s="5" t="str">
-        <f t="shared" ref="AR15:AR27" si="17">+IF(T15="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AR15:AR27" si="18">+IF(T15="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="AS15" s="5" t="str">
-        <f t="shared" ref="AS15:AS27" si="18">+IF(U15="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AS15:AS27" si="19">+IF(U15="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="AT15" s="5" t="str">
-        <f t="shared" ref="AT15:AT27" si="19">+IF(V15="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AT15:AT27" si="20">+IF(V15="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="AU15" s="5" t="str">
-        <f t="shared" ref="AU15:AU27" si="20">+IF(W15="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AU15:AU27" si="21">+IF(W15="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="AV15" s="5" t="str">
-        <f t="shared" ref="AV15:AV27" si="21">+IF(X15="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AV15:AV27" si="22">+IF(X15="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="AW15" s="5" t="str">
-        <f t="shared" ref="AW15:AW27" si="22">+IF(Y15="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AW15:AW27" si="23">+IF(Y15="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="AX15" s="5" t="str">
-        <f t="shared" ref="AX15:AX27" si="23">+IF(Z15="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AX15:AX27" si="24">+IF(Z15="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="AY15" s="5" t="str">
-        <f t="shared" ref="AY15:AY27" si="24">+IF(AA15="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AY15:AY27" si="25">+IF(AA15="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="AZ15" s="5" t="str">
-        <f t="shared" ref="AZ15:AZ27" si="25">+IF(AB15="",",0,0,0,0",",1,1,1,1")</f>
+        <f t="shared" ref="AZ15:AZ27" si="26">+IF(AB15="",",0,0,0,0",",1,1,1,1")</f>
         <v>,0,0,0,0</v>
       </c>
       <c r="BA15" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BB15" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BC15" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BD15" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BE15" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BF15" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BG15" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BH15" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BI15" s="5" t="str">
+        <f t="shared" si="13"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BJ15" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BB15" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BC15" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BD15" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BE15" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BF15" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BG15" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BH15" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BI15" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BJ15" s="22" t="str">
-        <f t="shared" si="3"/>
         <v>0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK15">
@@ -7130,7 +7235,13 @@
       <c r="C16" s="4">
         <v>4</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="D16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F16" s="5">
         <v>14</v>
       </c>
@@ -7214,103 +7325,103 @@
         <v>30</v>
       </c>
       <c r="AL16" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0,0,0,0</v>
       </c>
       <c r="AM16" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AN16" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AO16" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AP16" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AQ16" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AR16" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AS16" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AT16" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AU16" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AV16" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AW16" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AX16" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AY16" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AZ16" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BA16" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BB16" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BC16" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BD16" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BE16" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BF16" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BG16" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BH16" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BI16" s="5" t="str">
         <f t="shared" si="13"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AO16" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AP16" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AQ16" s="5" t="str">
-        <f t="shared" si="16"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AR16" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AS16" s="5" t="str">
-        <f t="shared" si="18"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AT16" s="5" t="str">
-        <f t="shared" si="19"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AU16" s="5" t="str">
-        <f t="shared" si="20"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AV16" s="5" t="str">
-        <f t="shared" si="21"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AW16" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AX16" s="5" t="str">
-        <f t="shared" si="23"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AY16" s="5" t="str">
-        <f t="shared" si="24"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AZ16" s="5" t="str">
-        <f t="shared" si="25"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BA16" s="5" t="str">
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BJ16" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BB16" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BC16" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BD16" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BE16" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BF16" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BG16" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BH16" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BI16" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BJ16" s="22" t="str">
-        <f t="shared" si="3"/>
         <v>0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK16">
@@ -7612,7 +7723,13 @@
       <c r="C17" s="4">
         <v>1</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="D17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="F17" s="5">
         <v>15</v>
       </c>
@@ -7696,103 +7813,103 @@
       <c r="AJ17" s="15"/>
       <c r="AK17" s="16"/>
       <c r="AL17" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0,0,0,0</v>
       </c>
       <c r="AM17" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AN17" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AO17" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AP17" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AQ17" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AR17" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AS17" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AT17" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AU17" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AV17" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AW17" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AX17" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AY17" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AZ17" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BA17" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BB17" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BC17" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BD17" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BE17" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BF17" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BG17" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BH17" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BI17" s="5" t="str">
         <f t="shared" si="13"/>
         <v>,0,0,0,0</v>
       </c>
-      <c r="AO17" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AP17" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AQ17" s="5" t="str">
-        <f t="shared" si="16"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AR17" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AS17" s="5" t="str">
-        <f t="shared" si="18"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AT17" s="5" t="str">
-        <f t="shared" si="19"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AU17" s="5" t="str">
-        <f t="shared" si="20"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AV17" s="5" t="str">
-        <f t="shared" si="21"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AW17" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AX17" s="5" t="str">
-        <f t="shared" si="23"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AY17" s="5" t="str">
-        <f t="shared" si="24"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AZ17" s="5" t="str">
-        <f t="shared" si="25"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BA17" s="5" t="str">
+      <c r="BJ17" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BB17" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BC17" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BD17" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BE17" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BF17" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BG17" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BH17" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BI17" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BJ17" s="22" t="str">
-        <f t="shared" si="3"/>
         <v>0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK17">
@@ -8094,7 +8211,13 @@
       <c r="C18" s="4">
         <v>1</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="D18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="F18" s="5">
         <v>16</v>
       </c>
@@ -8178,103 +8301,103 @@
       <c r="AJ18" s="15"/>
       <c r="AK18" s="16"/>
       <c r="AL18" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1,1,1,1</v>
       </c>
       <c r="AM18" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AN18" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AO18" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AP18" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AQ18" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AR18" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AS18" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AT18" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AU18" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AV18" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AW18" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AX18" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AY18" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AZ18" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BA18" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BB18" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BC18" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BD18" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BE18" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BF18" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BG18" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BH18" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BI18" s="5" t="str">
         <f t="shared" si="13"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AO18" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AP18" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AQ18" s="5" t="str">
-        <f t="shared" si="16"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AR18" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AS18" s="5" t="str">
-        <f t="shared" si="18"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AT18" s="5" t="str">
-        <f t="shared" si="19"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AU18" s="5" t="str">
-        <f t="shared" si="20"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AV18" s="5" t="str">
-        <f t="shared" si="21"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AW18" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AX18" s="5" t="str">
-        <f t="shared" si="23"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AY18" s="5" t="str">
-        <f t="shared" si="24"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AZ18" s="5" t="str">
-        <f t="shared" si="25"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BA18" s="5" t="str">
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BJ18" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BB18" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BC18" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BD18" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BE18" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BF18" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BG18" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BH18" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BI18" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BJ18" s="22" t="str">
-        <f t="shared" si="3"/>
         <v>1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,1,1,1,1,0,0,0,0,1,1,1,1,0,0,0,0,1,1,1,1,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,1,1,1,1,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK18">
@@ -8576,7 +8699,13 @@
       <c r="C19" s="4">
         <v>4</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="D19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F19" s="5">
         <v>17</v>
       </c>
@@ -8648,103 +8777,103 @@
       <c r="AJ19" s="15"/>
       <c r="AK19" s="16"/>
       <c r="AL19" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1,1,1,1</v>
       </c>
       <c r="AM19" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AN19" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AO19" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AP19" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AQ19" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AR19" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AS19" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AT19" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AU19" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AV19" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AW19" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AX19" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AY19" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AZ19" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BA19" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BB19" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BC19" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BD19" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BE19" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BF19" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BG19" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BH19" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BI19" s="5" t="str">
         <f t="shared" si="13"/>
         <v>,0,0,0,0</v>
       </c>
-      <c r="AO19" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AP19" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AQ19" s="5" t="str">
-        <f t="shared" si="16"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AR19" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AS19" s="5" t="str">
-        <f t="shared" si="18"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AT19" s="5" t="str">
-        <f t="shared" si="19"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AU19" s="5" t="str">
-        <f t="shared" si="20"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AV19" s="5" t="str">
-        <f t="shared" si="21"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AW19" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AX19" s="5" t="str">
-        <f t="shared" si="23"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AY19" s="5" t="str">
-        <f t="shared" si="24"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AZ19" s="5" t="str">
-        <f t="shared" si="25"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BA19" s="5" t="str">
+      <c r="BJ19" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BB19" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BC19" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BD19" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BE19" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BF19" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BG19" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BH19" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BI19" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BJ19" s="22" t="str">
-        <f t="shared" si="3"/>
         <v>1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK19">
@@ -9046,7 +9175,13 @@
       <c r="C20" s="4">
         <v>4</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="D20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="F20" s="5">
         <v>18</v>
       </c>
@@ -9140,103 +9275,103 @@
         <v>30</v>
       </c>
       <c r="AL20" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0,0,0,0</v>
       </c>
       <c r="AM20" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AN20" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AO20" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AP20" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AQ20" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AR20" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AS20" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AT20" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AU20" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AV20" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AW20" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AX20" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AY20" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AZ20" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BA20" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BB20" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BC20" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BD20" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BE20" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BF20" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BG20" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BH20" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BI20" s="5" t="str">
         <f t="shared" si="13"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AO20" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AP20" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AQ20" s="5" t="str">
-        <f t="shared" si="16"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AR20" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AS20" s="5" t="str">
-        <f t="shared" si="18"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AT20" s="5" t="str">
-        <f t="shared" si="19"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AU20" s="5" t="str">
-        <f t="shared" si="20"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AV20" s="5" t="str">
-        <f t="shared" si="21"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AW20" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AX20" s="5" t="str">
-        <f t="shared" si="23"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AY20" s="5" t="str">
-        <f t="shared" si="24"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AZ20" s="5" t="str">
-        <f t="shared" si="25"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BA20" s="5" t="str">
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BJ20" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BB20" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BC20" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BD20" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BE20" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BF20" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BG20" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BH20" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BI20" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BJ20" s="22" t="str">
-        <f t="shared" si="3"/>
         <v>0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK20">
@@ -9538,7 +9673,13 @@
       <c r="C21" s="4">
         <v>1</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="D21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="F21" s="5">
         <v>19</v>
       </c>
@@ -9628,103 +9769,103 @@
         <v>30</v>
       </c>
       <c r="AL21" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0,0,0,0</v>
       </c>
       <c r="AM21" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AN21" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AO21" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AP21" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AQ21" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AR21" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AS21" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AT21" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AU21" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AV21" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AW21" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AX21" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AY21" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AZ21" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BA21" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BB21" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BC21" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BD21" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BE21" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BF21" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BG21" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BH21" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BI21" s="5" t="str">
         <f t="shared" si="13"/>
         <v>,0,0,0,0</v>
       </c>
-      <c r="AO21" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AP21" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AQ21" s="5" t="str">
-        <f t="shared" si="16"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AR21" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AS21" s="5" t="str">
-        <f t="shared" si="18"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AT21" s="5" t="str">
-        <f t="shared" si="19"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AU21" s="5" t="str">
-        <f t="shared" si="20"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AV21" s="5" t="str">
-        <f t="shared" si="21"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AW21" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AX21" s="5" t="str">
-        <f t="shared" si="23"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AY21" s="5" t="str">
-        <f t="shared" si="24"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AZ21" s="5" t="str">
-        <f t="shared" si="25"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BA21" s="5" t="str">
+      <c r="BJ21" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BB21" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BC21" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BD21" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BE21" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BF21" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BG21" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BH21" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BI21" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BJ21" s="22" t="str">
-        <f t="shared" si="3"/>
         <v>0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK21">
@@ -10026,7 +10167,13 @@
       <c r="C22" s="4">
         <v>3</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="D22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="F22" s="5">
         <v>20</v>
       </c>
@@ -10120,103 +10267,103 @@
         <v>30</v>
       </c>
       <c r="AL22" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1,1,1,1</v>
       </c>
       <c r="AM22" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AN22" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AO22" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AP22" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AQ22" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AR22" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AS22" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AT22" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AU22" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AV22" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AW22" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AX22" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AY22" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AZ22" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BA22" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BB22" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BC22" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BD22" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BE22" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BF22" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BG22" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BH22" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BI22" s="5" t="str">
         <f t="shared" si="13"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AO22" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AP22" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AQ22" s="5" t="str">
-        <f t="shared" si="16"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AR22" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AS22" s="5" t="str">
-        <f t="shared" si="18"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AT22" s="5" t="str">
-        <f t="shared" si="19"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AU22" s="5" t="str">
-        <f t="shared" si="20"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AV22" s="5" t="str">
-        <f t="shared" si="21"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AW22" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AX22" s="5" t="str">
-        <f t="shared" si="23"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AY22" s="5" t="str">
-        <f t="shared" si="24"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AZ22" s="5" t="str">
-        <f t="shared" si="25"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BA22" s="5" t="str">
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BJ22" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BB22" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BC22" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BD22" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BE22" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BF22" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BG22" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BH22" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BI22" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BJ22" s="22" t="str">
-        <f t="shared" si="3"/>
         <v>1,1,1,1,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK22">
@@ -10579,103 +10726,103 @@
       <c r="AJ23" s="15"/>
       <c r="AK23" s="16"/>
       <c r="AL23" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1,1,1,1</v>
       </c>
       <c r="AM23" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AN23" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AO23" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AP23" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AQ23" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AR23" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AS23" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AT23" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AU23" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AV23" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AW23" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AX23" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AY23" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AZ23" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BA23" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BB23" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BC23" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BD23" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BE23" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BF23" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BG23" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BH23" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BI23" s="5" t="str">
         <f t="shared" si="13"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AO23" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AP23" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AQ23" s="5" t="str">
-        <f t="shared" si="16"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AR23" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AS23" s="5" t="str">
-        <f t="shared" si="18"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AT23" s="5" t="str">
-        <f t="shared" si="19"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AU23" s="5" t="str">
-        <f t="shared" si="20"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AV23" s="5" t="str">
-        <f t="shared" si="21"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AW23" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AX23" s="5" t="str">
-        <f t="shared" si="23"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AY23" s="5" t="str">
-        <f t="shared" si="24"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AZ23" s="5" t="str">
-        <f t="shared" si="25"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BA23" s="5" t="str">
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BJ23" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BB23" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BC23" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BD23" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BE23" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BF23" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BG23" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BH23" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BI23" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BJ23" s="22" t="str">
-        <f t="shared" si="3"/>
         <v>1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK23">
@@ -11034,103 +11181,103 @@
       <c r="AJ24" s="15"/>
       <c r="AK24" s="16"/>
       <c r="AL24" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1,1,1,1</v>
       </c>
       <c r="AM24" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AN24" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AO24" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AP24" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AQ24" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AR24" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AS24" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AT24" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AU24" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AV24" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AW24" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AX24" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AY24" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AZ24" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BA24" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BB24" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BC24" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BD24" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BE24" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BF24" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BG24" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BH24" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BI24" s="5" t="str">
         <f t="shared" si="13"/>
         <v>,0,0,0,0</v>
       </c>
-      <c r="AO24" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AP24" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AQ24" s="5" t="str">
-        <f t="shared" si="16"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AR24" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AS24" s="5" t="str">
-        <f t="shared" si="18"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AT24" s="5" t="str">
-        <f t="shared" si="19"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AU24" s="5" t="str">
-        <f t="shared" si="20"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AV24" s="5" t="str">
-        <f t="shared" si="21"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AW24" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AX24" s="5" t="str">
-        <f t="shared" si="23"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AY24" s="5" t="str">
-        <f t="shared" si="24"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AZ24" s="5" t="str">
-        <f t="shared" si="25"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BA24" s="5" t="str">
+      <c r="BJ24" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BB24" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BC24" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BD24" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BE24" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BF24" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BG24" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BH24" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BI24" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BJ24" s="22" t="str">
-        <f t="shared" si="3"/>
         <v>1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK24">
@@ -11517,103 +11664,103 @@
         <v>30</v>
       </c>
       <c r="AL25" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0,0,0,0</v>
       </c>
       <c r="AM25" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AN25" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AO25" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AP25" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AQ25" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AR25" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AS25" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AT25" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AU25" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AV25" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AW25" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AX25" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AY25" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AZ25" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BA25" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BB25" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BC25" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BD25" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BE25" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BF25" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BG25" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BH25" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BI25" s="5" t="str">
         <f t="shared" si="13"/>
         <v>,0,0,0,0</v>
       </c>
-      <c r="AO25" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AP25" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AQ25" s="5" t="str">
-        <f t="shared" si="16"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AR25" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AS25" s="5" t="str">
-        <f t="shared" si="18"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AT25" s="5" t="str">
-        <f t="shared" si="19"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AU25" s="5" t="str">
-        <f t="shared" si="20"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AV25" s="5" t="str">
-        <f t="shared" si="21"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AW25" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AX25" s="5" t="str">
-        <f t="shared" si="23"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AY25" s="5" t="str">
-        <f t="shared" si="24"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AZ25" s="5" t="str">
-        <f t="shared" si="25"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BA25" s="5" t="str">
+      <c r="BJ25" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BB25" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BC25" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BD25" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BE25" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BF25" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BG25" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BH25" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BI25" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BJ25" s="22" t="str">
-        <f t="shared" si="3"/>
         <v>0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK25">
@@ -11990,103 +12137,103 @@
       <c r="AJ26" s="15"/>
       <c r="AK26" s="16"/>
       <c r="AL26" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0,0,0,0</v>
       </c>
       <c r="AM26" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,0,0,0,0</v>
       </c>
       <c r="AN26" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AO26" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AP26" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AQ26" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AR26" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AS26" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AT26" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AU26" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AV26" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AW26" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AX26" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AY26" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AZ26" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BA26" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="BB26" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BC26" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BD26" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BE26" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BF26" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BG26" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BH26" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BI26" s="5" t="str">
         <f t="shared" si="13"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AO26" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AP26" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AQ26" s="5" t="str">
-        <f t="shared" si="16"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AR26" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AS26" s="5" t="str">
-        <f t="shared" si="18"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AT26" s="5" t="str">
-        <f t="shared" si="19"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AU26" s="5" t="str">
-        <f t="shared" si="20"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AV26" s="5" t="str">
-        <f t="shared" si="21"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AW26" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AX26" s="5" t="str">
-        <f t="shared" si="23"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AY26" s="5" t="str">
-        <f t="shared" si="24"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AZ26" s="5" t="str">
-        <f t="shared" si="25"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BA26" s="5" t="str">
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BJ26" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="BB26" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BC26" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BD26" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BE26" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BF26" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BG26" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BH26" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BI26" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BJ26" s="22" t="str">
-        <f t="shared" si="3"/>
         <v>0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK26">
@@ -12441,103 +12588,103 @@
       <c r="AJ27" s="20"/>
       <c r="AK27" s="21"/>
       <c r="AL27" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1,1,1,1</v>
       </c>
       <c r="AM27" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>,1,1,1,1</v>
       </c>
       <c r="AN27" s="5" t="str">
+        <f t="shared" si="14"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AO27" s="5" t="str">
+        <f t="shared" si="15"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AP27" s="5" t="str">
+        <f t="shared" si="16"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AQ27" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AR27" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AS27" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>,1,1,1,1</v>
+      </c>
+      <c r="AT27" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AU27" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AV27" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AW27" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AX27" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AY27" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="AZ27" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BA27" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BB27" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BC27" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BD27" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BE27" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BF27" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BG27" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BH27" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BI27" s="5" t="str">
         <f t="shared" si="13"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AO27" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AP27" s="5" t="str">
-        <f t="shared" si="15"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AQ27" s="5" t="str">
-        <f t="shared" si="16"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AR27" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AS27" s="5" t="str">
-        <f t="shared" si="18"/>
-        <v>,1,1,1,1</v>
-      </c>
-      <c r="AT27" s="5" t="str">
-        <f t="shared" si="19"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AU27" s="5" t="str">
-        <f t="shared" si="20"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AV27" s="5" t="str">
-        <f t="shared" si="21"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AW27" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AX27" s="5" t="str">
-        <f t="shared" si="23"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AY27" s="5" t="str">
-        <f t="shared" si="24"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="AZ27" s="5" t="str">
-        <f t="shared" si="25"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BA27" s="5" t="str">
+        <v>,0,0,0,0</v>
+      </c>
+      <c r="BJ27" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BB27" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BC27" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BD27" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BE27" s="5" t="str">
-        <f t="shared" si="8"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BF27" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BG27" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BH27" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BI27" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>,0,0,0,0</v>
-      </c>
-      <c r="BJ27" s="22" t="str">
-        <f t="shared" si="3"/>
         <v>1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,0,0,0,0,0,0,1,1,1,1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="BK27">
@@ -12838,26 +12985,42 @@
     <row r="29" spans="1:158" x14ac:dyDescent="0.25">
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
+      <c r="G29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:158" x14ac:dyDescent="0.25">
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+      <c r="G30" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="1:158" x14ac:dyDescent="0.25">
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
+      <c r="G31" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:158" x14ac:dyDescent="0.25">
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="33" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E33" s="4"/>
@@ -13014,5 +13177,6 @@
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>